<commit_message>
rebalansovanie pridanie starych cien
</commit_message>
<xml_diff>
--- a/buying_info/rebalansovanie.xlsx
+++ b/buying_info/rebalansovanie.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rados\Desktop\financna\buying_info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0AB529C8-EDEE-4037-88B8-08BC42107D79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D08E626-B2C2-4AB1-AA94-B61E9B2D69FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{7730A6B8-4958-445F-A23A-A395ABB50691}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="80">
   <si>
     <t>Symbol</t>
   </si>
@@ -268,6 +268,12 @@
   </si>
   <si>
     <t>inv. reb. 12.12.</t>
+  </si>
+  <si>
+    <t>ks akcie 1.12.</t>
+  </si>
+  <si>
+    <t>cena akcie 1.12.</t>
   </si>
 </sst>
 </file>
@@ -275,7 +281,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.000000"/>
+    <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -403,7 +409,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -427,18 +433,18 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="1" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -447,6 +453,7 @@
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normálna" xfId="0" builtinId="0"/>
@@ -766,10 +773,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C06B7A6-18C0-4EEF-BAC0-8E9C65C53C40}">
-  <dimension ref="A1:U44"/>
+  <dimension ref="A1:W44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -777,25 +784,27 @@
     <col min="1" max="1" width="18.1796875" customWidth="1"/>
     <col min="2" max="2" width="8.7265625" style="1"/>
     <col min="3" max="3" width="10.7265625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="17.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.26953125" customWidth="1"/>
-    <col min="9" max="9" width="8.36328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18" customWidth="1"/>
-    <col min="14" max="14" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.36328125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.7265625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.08984375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.1796875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="21.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.26953125" customWidth="1"/>
+    <col min="11" max="11" width="8.36328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18" customWidth="1"/>
+    <col min="16" max="16" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="21.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>43</v>
       </c>
@@ -805,59 +814,65 @@
       <c r="C1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F1" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="I1" s="22" t="s">
+      <c r="K1" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="J1" s="22" t="s">
+      <c r="L1" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="W1" s="4" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>44</v>
       </c>
@@ -867,68 +882,75 @@
       <c r="C2" s="32">
         <v>12885.08</v>
       </c>
-      <c r="D2" s="23">
+      <c r="D2" s="32">
+        <v>142</v>
+      </c>
+      <c r="E2" s="32">
+        <f>C2/D2</f>
+        <v>90.74</v>
+      </c>
+      <c r="F2" s="23">
         <v>14573.46</v>
       </c>
-      <c r="E2" s="23">
-        <f>D2-C2</f>
+      <c r="G2" s="23">
+        <f t="shared" ref="G2:G43" si="0">F2-C2</f>
         <v>1688.3799999999992</v>
       </c>
-      <c r="F2">
+      <c r="H2">
         <v>102.63</v>
       </c>
-      <c r="G2">
+      <c r="I2">
         <v>8</v>
       </c>
-      <c r="H2">
-        <f>G2*F2</f>
+      <c r="J2">
+        <f>I2*H2</f>
         <v>821.04</v>
       </c>
-      <c r="I2" s="20"/>
-      <c r="J2" s="17">
+      <c r="K2" s="20"/>
+      <c r="L2" s="17">
         <v>821.04</v>
       </c>
-      <c r="K2">
-        <f>D2-(F2*G2)</f>
+      <c r="M2">
+        <f>F2-(H2*I2)</f>
         <v>13752.419999999998</v>
       </c>
-      <c r="M2" s="23" t="s">
+      <c r="O2" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="N2" s="24">
+      <c r="P2" s="24">
         <f>C2+C4+C12+C13+C26+C29+C31</f>
         <v>30396.25</v>
       </c>
-      <c r="O2" s="25">
-        <f>N2/$N$12*100</f>
-        <v>30.610650054043532</v>
-      </c>
-      <c r="P2" s="24">
-        <f>D2+D4+D12+D13+D26+D29+D31</f>
-        <v>32309.61</v>
-      </c>
       <c r="Q2" s="25">
         <f>P2/$P$12*100</f>
+        <v>30.610650054043532</v>
+      </c>
+      <c r="R2" s="24">
+        <f>F2+F4+F12+F13+F26+F29+F31</f>
+        <v>32309.61</v>
+      </c>
+      <c r="S2" s="25">
+        <f t="shared" ref="S2:S11" si="1">R2/$R$12*100</f>
         <v>31.367566690135192</v>
       </c>
-      <c r="R2" s="26">
-        <f>Q2-O2</f>
+      <c r="T2" s="26">
+        <f t="shared" ref="T2:T11" si="2">S2-Q2</f>
         <v>0.75691663609165971</v>
       </c>
-      <c r="S2" s="23">
-        <f>K2+K4+K12+K13+K26+K29+K31</f>
+      <c r="U2" s="23">
+        <f>M2+M4+M12+M13+M26+M29+M31</f>
         <v>31488.57</v>
       </c>
-      <c r="T2" s="25">
-        <f>S2/$S$12*100</f>
+      <c r="V2" s="25">
+        <f>U2/$U$12*100</f>
         <v>30.561321178647145</v>
       </c>
-      <c r="U2" s="26">
-        <f>T2-O2</f>
+      <c r="W2" s="26">
+        <f t="shared" ref="W2:W11" si="3">V2-Q2</f>
         <v>-4.9328875396387417E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>45</v>
       </c>
@@ -938,72 +960,79 @@
       <c r="C3" s="34">
         <v>10417.68</v>
       </c>
-      <c r="D3" s="27">
+      <c r="D3" s="34">
+        <v>42</v>
+      </c>
+      <c r="E3" s="34">
+        <f t="shared" ref="E3:E43" si="4">C3/D3</f>
+        <v>248.04000000000002</v>
+      </c>
+      <c r="F3" s="27">
         <v>10253.879999999999</v>
       </c>
-      <c r="E3" s="27">
-        <f>D3-C3</f>
+      <c r="G3" s="27">
+        <f t="shared" si="0"/>
         <v>-163.80000000000109</v>
       </c>
-      <c r="F3">
+      <c r="H3">
         <v>244.14</v>
       </c>
-      <c r="G3">
-        <f>-ROUND(H3/F3, 1)</f>
+      <c r="I3">
+        <f>-ROUND(J3/H3, 1)</f>
         <v>2</v>
       </c>
-      <c r="H3">
-        <f>-$H$2*I3</f>
+      <c r="J3">
+        <f>-$J$2*K3</f>
         <v>-480.96113296617091</v>
       </c>
-      <c r="I3" s="20">
-        <f>E3/($E$3+$E$5+$E$6+$E$7)</f>
+      <c r="K3" s="20">
+        <f>G3/($G$3+$G$5+$G$6+$G$7)</f>
         <v>0.58579500751019553</v>
       </c>
-      <c r="J3" s="17">
+      <c r="L3" s="17">
         <v>-488.28</v>
       </c>
-      <c r="K3">
-        <f>D3+(F3*G3)</f>
+      <c r="M3">
+        <f>F3+(H3*I3)</f>
         <v>10742.16</v>
       </c>
-      <c r="M3" s="27" t="s">
+      <c r="O3" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="N3" s="28">
+      <c r="P3" s="28">
         <f>C3+C5+C7+C15+C43</f>
         <v>19794.099999999999</v>
       </c>
-      <c r="O3" s="29">
-        <f t="shared" ref="O3:O11" si="0">N3/$N$12*100</f>
+      <c r="Q3" s="29">
+        <f t="shared" ref="Q3:Q11" si="5">P3/$P$12*100</f>
         <v>19.933717752510361</v>
       </c>
-      <c r="P3" s="28">
-        <f>D3+D5+D7+D15+D43</f>
+      <c r="R3" s="28">
+        <f>F3+F5+F7+F15+F43</f>
         <v>19712.970000000005</v>
       </c>
-      <c r="Q3" s="29">
-        <f>P3/$P$12*100</f>
+      <c r="S3" s="29">
+        <f t="shared" si="1"/>
         <v>19.138203807957897</v>
       </c>
-      <c r="R3" s="30">
-        <f>Q3-O3</f>
+      <c r="T3" s="30">
+        <f t="shared" si="2"/>
         <v>-0.79551394455246438</v>
       </c>
-      <c r="S3" s="27">
-        <f>K3+K5+K7+K15+K43</f>
+      <c r="U3" s="27">
+        <f>M3+M5+M7+M15+M43</f>
         <v>20412.410000000003</v>
       </c>
-      <c r="T3" s="29">
-        <f t="shared" ref="T3:T11" si="1">S3/$S$12*100</f>
+      <c r="V3" s="29">
+        <f t="shared" ref="V3:V11" si="6">U3/$U$12*100</f>
         <v>19.811322585948769</v>
       </c>
-      <c r="U3" s="30">
-        <f>T3-O3</f>
+      <c r="W3" s="30">
+        <f t="shared" si="3"/>
         <v>-0.12239516656159211</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>44</v>
       </c>
@@ -1013,55 +1042,62 @@
       <c r="C4" s="1">
         <v>8264.75</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
+        <v>25</v>
+      </c>
+      <c r="E4" s="35">
+        <f t="shared" si="4"/>
+        <v>330.59</v>
+      </c>
+      <c r="F4">
         <v>8563.5</v>
       </c>
-      <c r="E4">
-        <f>D4-C4</f>
+      <c r="G4">
+        <f t="shared" si="0"/>
         <v>298.75</v>
       </c>
-      <c r="I4" s="20"/>
-      <c r="J4" s="17"/>
-      <c r="K4">
+      <c r="K4" s="20"/>
+      <c r="L4" s="17"/>
+      <c r="M4">
         <v>8563.5</v>
       </c>
-      <c r="M4" s="27" t="s">
+      <c r="O4" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="N4" s="28">
+      <c r="P4" s="28">
         <f>C22+C6</f>
         <v>5047</v>
       </c>
-      <c r="O4" s="29">
-        <f t="shared" si="0"/>
+      <c r="Q4" s="29">
+        <f t="shared" si="5"/>
         <v>5.0825990318791865</v>
       </c>
-      <c r="P4" s="28">
-        <f>D22+D6</f>
+      <c r="R4" s="28">
+        <f>F22+F6</f>
         <v>5108.8100000000004</v>
       </c>
-      <c r="Q4" s="29">
-        <f>P4/$P$12*100</f>
+      <c r="S4" s="29">
+        <f t="shared" si="1"/>
         <v>4.9598536900392665</v>
       </c>
-      <c r="R4" s="30">
-        <f>Q4-O4</f>
+      <c r="T4" s="30">
+        <f t="shared" si="2"/>
         <v>-0.12274534183992003</v>
       </c>
-      <c r="S4" s="27">
-        <f>K22+K6</f>
+      <c r="U4" s="27">
+        <f>M22+M6</f>
         <v>5261.2300000000005</v>
       </c>
-      <c r="T4" s="29">
-        <f t="shared" si="1"/>
+      <c r="V4" s="29">
+        <f t="shared" si="6"/>
         <v>5.1063017413853258</v>
       </c>
-      <c r="U4" s="30">
-        <f>T4-O4</f>
+      <c r="W4" s="30">
+        <f t="shared" si="3"/>
         <v>2.3702709506139286E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>45</v>
       </c>
@@ -1071,72 +1107,79 @@
       <c r="C5" s="34">
         <v>3761.1</v>
       </c>
-      <c r="D5" s="27">
+      <c r="D5" s="34">
+        <v>70</v>
+      </c>
+      <c r="E5" s="34">
+        <f t="shared" si="4"/>
+        <v>53.73</v>
+      </c>
+      <c r="F5" s="27">
         <v>3695.3</v>
       </c>
-      <c r="E5" s="27">
-        <f>D5-C5</f>
+      <c r="G5" s="27">
+        <f t="shared" si="0"/>
         <v>-65.799999999999727</v>
       </c>
-      <c r="F5">
+      <c r="H5">
         <v>52.79</v>
       </c>
-      <c r="G5">
-        <f>-ROUND(H5/F5, 0)</f>
+      <c r="I5">
+        <f>-ROUND(J5/H5, 0)</f>
         <v>4</v>
       </c>
-      <c r="H5">
-        <f>-$H$2*I5</f>
+      <c r="J5">
+        <f>-$J$2*K5</f>
         <v>-193.20660896931443</v>
       </c>
-      <c r="I5" s="20">
-        <f>E5/($E$3+$E$5+$E$6+$E$7)</f>
+      <c r="K5" s="20">
+        <f>G5/($G$3+$G$5+$G$6+$G$7)</f>
         <v>0.2353193619912726</v>
       </c>
-      <c r="J5" s="17">
+      <c r="L5" s="17">
         <v>-211.16</v>
       </c>
-      <c r="K5">
-        <f>D5+(F5*G5)</f>
+      <c r="M5">
+        <f>F5+(H5*I5)</f>
         <v>3906.46</v>
       </c>
-      <c r="M5" t="s">
+      <c r="O5" t="s">
         <v>54</v>
       </c>
-      <c r="N5" s="17">
+      <c r="P5" s="17">
         <f>C8+C14+C16+C17+C38</f>
         <v>10640.14</v>
       </c>
-      <c r="O5" s="19">
-        <f t="shared" si="0"/>
+      <c r="Q5" s="19">
+        <f t="shared" si="5"/>
         <v>10.715190264128987</v>
       </c>
-      <c r="P5" s="17">
-        <f>D8+D14+D16+D17+D38</f>
+      <c r="R5" s="17">
+        <f>F8+F14+F16+F17+F38</f>
         <v>10986.4</v>
       </c>
-      <c r="Q5" s="19">
-        <f>P5/$P$12*100</f>
+      <c r="S5" s="19">
+        <f t="shared" si="1"/>
         <v>10.666072251707813</v>
       </c>
-      <c r="R5" s="20">
-        <f>Q5-O5</f>
+      <c r="T5" s="20">
+        <f t="shared" si="2"/>
         <v>-4.9118012421173418E-2</v>
       </c>
-      <c r="S5">
-        <f>K8+K14+K16+K17+K38</f>
+      <c r="U5">
+        <f>M8+M14+M16+M17+M38</f>
         <v>10986.4</v>
       </c>
-      <c r="T5" s="22">
-        <f t="shared" si="1"/>
+      <c r="V5" s="22">
+        <f t="shared" si="6"/>
         <v>10.662881769387717</v>
       </c>
-      <c r="U5" s="20">
-        <f>T5-O5</f>
+      <c r="W5" s="20">
+        <f t="shared" si="3"/>
         <v>-5.2308494741270195E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A6" s="13" t="s">
         <v>47</v>
       </c>
@@ -1146,71 +1189,78 @@
       <c r="C6" s="34">
         <v>3209.64</v>
       </c>
-      <c r="D6" s="27">
+      <c r="D6" s="34">
+        <v>21</v>
+      </c>
+      <c r="E6" s="34">
+        <f t="shared" si="4"/>
+        <v>152.84</v>
+      </c>
+      <c r="F6" s="27">
         <v>3200.82</v>
       </c>
-      <c r="E6" s="27">
-        <f>D6-C6</f>
+      <c r="G6" s="27">
+        <f t="shared" si="0"/>
         <v>-8.819999999999709</v>
       </c>
-      <c r="F6">
+      <c r="H6">
         <v>152.41999999999999</v>
       </c>
-      <c r="G6">
+      <c r="I6">
         <v>1</v>
       </c>
-      <c r="H6">
-        <f>-$H$2*I6</f>
+      <c r="J6">
+        <f>-$J$2*K6</f>
         <v>-25.897907159715871</v>
       </c>
-      <c r="I6" s="20">
-        <f>E6/($E$3+$E$5+$E$6+$E$7)</f>
+      <c r="K6" s="20">
+        <f>G6/($G$3+$G$5+$G$6+$G$7)</f>
         <v>3.154280809670159E-2</v>
       </c>
-      <c r="J6" s="17">
+      <c r="L6" s="17">
         <v>-152.41999999999999</v>
       </c>
-      <c r="K6">
-        <f>D6+(F6*G6)</f>
+      <c r="M6">
+        <f>F6+(H6*I6)</f>
         <v>3353.2400000000002</v>
       </c>
-      <c r="M6" t="s">
+      <c r="O6" t="s">
         <v>55</v>
       </c>
-      <c r="N6" s="17">
+      <c r="P6" s="17">
         <f>C10+C23+C42</f>
         <v>4746.22</v>
       </c>
-      <c r="O6" s="19">
-        <f t="shared" si="0"/>
+      <c r="Q6" s="19">
+        <f t="shared" si="5"/>
         <v>4.7796974791134597</v>
       </c>
-      <c r="P6" s="17">
-        <f>D10+D23+D42</f>
+      <c r="R6" s="17">
+        <f>F10+F23+F42</f>
         <v>4923.12</v>
       </c>
-      <c r="Q6" s="19">
-        <f>P6/$P$12*100</f>
+      <c r="S6" s="19">
+        <f t="shared" si="1"/>
         <v>4.7795778074553787</v>
       </c>
-      <c r="R6" s="20">
-        <f>Q6-O6</f>
+      <c r="T6" s="20">
+        <f t="shared" si="2"/>
         <v>-1.1967165808091096E-4</v>
       </c>
-      <c r="S6">
-        <f>K10+K23+K42</f>
+      <c r="U6">
+        <f>M10+M23+M42</f>
         <v>4923.12</v>
       </c>
-      <c r="T6" s="22">
-        <f t="shared" si="1"/>
+      <c r="V6" s="22">
+        <f t="shared" si="6"/>
         <v>4.7781481191753485</v>
       </c>
-      <c r="U6" s="20">
-        <f>T6-O6</f>
+      <c r="W6" s="20">
+        <f t="shared" si="3"/>
         <v>-1.5493599381111167E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
         <v>45</v>
       </c>
@@ -1220,72 +1270,79 @@
       <c r="C7" s="34">
         <v>3216.1</v>
       </c>
-      <c r="D7" s="27">
+      <c r="D7" s="34">
+        <v>10</v>
+      </c>
+      <c r="E7" s="34">
+        <f t="shared" si="4"/>
+        <v>321.61</v>
+      </c>
+      <c r="F7" s="27">
         <v>3174.9</v>
       </c>
-      <c r="E7" s="27">
-        <f>D7-C7</f>
+      <c r="G7" s="27">
+        <f t="shared" si="0"/>
         <v>-41.199999999999818</v>
       </c>
-      <c r="F7">
+      <c r="H7">
         <v>317.49</v>
       </c>
-      <c r="G7">
-        <f>-ROUND(H7/F7, 0)</f>
+      <c r="I7">
+        <f>-ROUND(J7/H7, 0)</f>
         <v>0</v>
       </c>
-      <c r="H7">
-        <f>-$H$2*I7</f>
+      <c r="J7">
+        <f>-$J$2*K7</f>
         <v>-120.97435090479868</v>
       </c>
-      <c r="I7" s="20">
-        <f>E7/($E$3+$E$5+$E$6+$E$7)</f>
+      <c r="K7" s="20">
+        <f>G7/($G$3+$G$5+$G$6+$G$7)</f>
         <v>0.14734282240183022</v>
       </c>
-      <c r="J7" s="17">
+      <c r="L7" s="17">
         <v>0</v>
       </c>
-      <c r="K7">
-        <f>D7+(F7*G7)</f>
+      <c r="M7">
+        <f>F7+(H7*I7)</f>
         <v>3174.9</v>
       </c>
-      <c r="M7" t="s">
+      <c r="O7" t="s">
         <v>49</v>
       </c>
-      <c r="N7" s="17">
+      <c r="P7" s="17">
         <f>C25</f>
         <v>2849.04</v>
       </c>
-      <c r="O7" s="19">
-        <f t="shared" si="0"/>
+      <c r="Q7" s="19">
+        <f t="shared" si="5"/>
         <v>2.8691357134505795</v>
       </c>
-      <c r="P7" s="17">
-        <f>D25</f>
+      <c r="R7" s="17">
+        <f>F25</f>
         <v>2973.5</v>
       </c>
-      <c r="Q7" s="19">
-        <f>P7/$P$12*100</f>
+      <c r="S7" s="19">
+        <f t="shared" si="1"/>
         <v>2.8868023957304652</v>
       </c>
-      <c r="R7" s="20">
-        <f>Q7-O7</f>
+      <c r="T7" s="20">
+        <f t="shared" si="2"/>
         <v>1.7666682279885659E-2</v>
       </c>
-      <c r="S7">
-        <f>K25</f>
+      <c r="U7">
+        <f>M25</f>
         <v>2973.5</v>
       </c>
-      <c r="T7" s="22">
-        <f t="shared" si="1"/>
+      <c r="V7" s="22">
+        <f t="shared" si="6"/>
         <v>2.8859388827345058</v>
       </c>
-      <c r="U7" s="20">
-        <f>T7-O7</f>
+      <c r="W7" s="20">
+        <f t="shared" si="3"/>
         <v>1.6803169283926334E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A8" s="8" t="s">
         <v>51</v>
       </c>
@@ -1295,54 +1352,61 @@
       <c r="C8" s="1">
         <v>3127.97</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="1">
+        <v>163</v>
+      </c>
+      <c r="E8" s="35">
+        <f t="shared" si="4"/>
+        <v>19.189999999999998</v>
+      </c>
+      <c r="F8">
         <v>3496.35</v>
       </c>
-      <c r="E8">
-        <f>D8-C8</f>
+      <c r="G8">
+        <f t="shared" si="0"/>
         <v>368.38000000000011</v>
       </c>
-      <c r="J8" s="17"/>
-      <c r="K8">
+      <c r="L8" s="17"/>
+      <c r="M8">
         <v>3496.35</v>
       </c>
-      <c r="M8" s="5" t="s">
+      <c r="O8" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="N8" s="18">
+      <c r="P8" s="18">
         <f>C9+C35+C40</f>
         <v>4497.03</v>
       </c>
-      <c r="O8" s="19">
-        <f t="shared" si="0"/>
+      <c r="Q8" s="19">
+        <f t="shared" si="5"/>
         <v>4.5287498165903814</v>
       </c>
-      <c r="P8" s="18">
-        <f>D9+D35+D40</f>
+      <c r="R8" s="18">
+        <f>F9+F35+F40</f>
         <v>4832.1099999999997</v>
       </c>
-      <c r="Q8" s="19">
-        <f>P8/$P$12*100</f>
+      <c r="S8" s="19">
+        <f t="shared" si="1"/>
         <v>4.6912213635221578</v>
       </c>
-      <c r="R8" s="21">
-        <f>Q8-O8</f>
+      <c r="T8" s="21">
+        <f t="shared" si="2"/>
         <v>0.16247154693177634</v>
       </c>
-      <c r="S8" s="5">
-        <f>K9+K35+K40</f>
+      <c r="U8" s="5">
+        <f>M9+M35+M40</f>
         <v>4832.1099999999997</v>
       </c>
-      <c r="T8" s="22">
-        <f t="shared" si="1"/>
+      <c r="V8" s="22">
+        <f t="shared" si="6"/>
         <v>4.689818104809226</v>
       </c>
-      <c r="U8" s="20">
-        <f>T8-O8</f>
+      <c r="W8" s="20">
+        <f t="shared" si="3"/>
         <v>0.16106828821884456</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A9" s="10" t="s">
         <v>46</v>
       </c>
@@ -1352,53 +1416,60 @@
       <c r="C9" s="1">
         <v>3023.52</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="1">
+        <v>16</v>
+      </c>
+      <c r="E9" s="35">
+        <f t="shared" si="4"/>
+        <v>188.97</v>
+      </c>
+      <c r="F9">
         <v>3278.88</v>
       </c>
-      <c r="E9">
-        <f>D9-C9</f>
+      <c r="G9">
+        <f t="shared" si="0"/>
         <v>255.36000000000013</v>
       </c>
-      <c r="K9">
+      <c r="M9">
         <v>3278.88</v>
       </c>
-      <c r="M9" t="s">
+      <c r="O9" t="s">
         <v>48</v>
       </c>
-      <c r="N9" s="17">
+      <c r="P9" s="17">
         <f>C11+C19+C28</f>
         <v>6110.6</v>
       </c>
-      <c r="O9" s="19">
-        <f t="shared" si="0"/>
+      <c r="Q9" s="19">
+        <f t="shared" si="5"/>
         <v>6.1537011381416598</v>
       </c>
-      <c r="P9" s="17">
-        <f>D11+D19+D28</f>
+      <c r="R9" s="17">
+        <f>F11+F19+F28</f>
         <v>6410.43</v>
       </c>
-      <c r="Q9" s="19">
-        <f>P9/$P$12*100</f>
+      <c r="S9" s="19">
+        <f t="shared" si="1"/>
         <v>6.2235226775390773</v>
       </c>
-      <c r="R9" s="20">
-        <f>Q9-O9</f>
+      <c r="T9" s="20">
+        <f t="shared" si="2"/>
         <v>6.9821539397417531E-2</v>
       </c>
-      <c r="S9">
-        <f>K11+K19+K28</f>
+      <c r="U9">
+        <f>M11+M19+M28</f>
         <v>6410.43</v>
       </c>
-      <c r="T9" s="22">
-        <f t="shared" si="1"/>
+      <c r="V9" s="22">
+        <f t="shared" si="6"/>
         <v>6.2216610701354496</v>
       </c>
-      <c r="U9" s="20">
-        <f>T9-O9</f>
+      <c r="W9" s="20">
+        <f t="shared" si="3"/>
         <v>6.7959931993789802E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
         <v>50</v>
       </c>
@@ -1408,53 +1479,60 @@
       <c r="C10" s="1">
         <v>2696.9</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="1">
+        <v>5</v>
+      </c>
+      <c r="E10" s="35">
+        <f t="shared" si="4"/>
+        <v>539.38</v>
+      </c>
+      <c r="F10">
         <v>2794.1</v>
       </c>
-      <c r="E10">
-        <f>D10-C10</f>
+      <c r="G10">
+        <f t="shared" si="0"/>
         <v>97.199999999999818</v>
       </c>
-      <c r="K10">
+      <c r="M10">
         <v>2794.1</v>
       </c>
-      <c r="M10" t="s">
+      <c r="O10" t="s">
         <v>52</v>
       </c>
-      <c r="N10" s="17">
+      <c r="P10" s="17">
         <f>C18+C24+C27+C30+C32+C33+C34+C36+C37+C39+C41+C21</f>
         <v>13320.929999999998</v>
       </c>
-      <c r="O10" s="19">
-        <f t="shared" si="0"/>
+      <c r="Q10" s="19">
+        <f t="shared" si="5"/>
         <v>13.414889225625201</v>
       </c>
-      <c r="P10" s="17">
-        <f>D18+D24+D27+D30+D32+D33+D34+D36+D37+D39+D41+D21</f>
+      <c r="R10" s="17">
+        <f>F18+F24+F27+F30+F32+F33+F34+F36+F37+F39+F41+F21</f>
         <v>13805.529999999997</v>
       </c>
-      <c r="Q10" s="19">
-        <f>P10/$P$12*100</f>
+      <c r="S10" s="19">
+        <f t="shared" si="1"/>
         <v>13.4030055753586</v>
       </c>
-      <c r="R10" s="20">
-        <f>Q10-O10</f>
+      <c r="T10" s="20">
+        <f t="shared" si="2"/>
         <v>-1.1883650266600654E-2</v>
       </c>
-      <c r="S10">
-        <f>K18+K24+K27+K30+K32+K33+K34+K36+K37+K39+K41+K21</f>
+      <c r="U10">
+        <f>M18+M24+M27+M30+M32+M33+M34+M36+M37+M39+M41+M21</f>
         <v>13805.529999999997</v>
       </c>
-      <c r="T10" s="22">
-        <f t="shared" si="1"/>
+      <c r="V10" s="22">
+        <f t="shared" si="6"/>
         <v>13.398996409536807</v>
       </c>
-      <c r="U10" s="20">
-        <f>T10-O10</f>
+      <c r="W10" s="20">
+        <f t="shared" si="3"/>
         <v>-1.5892816088394213E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A11" s="12" t="s">
         <v>48</v>
       </c>
@@ -1464,53 +1542,60 @@
       <c r="C11" s="1">
         <v>2875.33</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="1">
+        <v>41</v>
+      </c>
+      <c r="E11" s="35">
+        <f t="shared" si="4"/>
+        <v>70.13</v>
+      </c>
+      <c r="F11">
         <v>3013.09</v>
       </c>
-      <c r="E11">
-        <f>D11-C11</f>
+      <c r="G11">
+        <f t="shared" si="0"/>
         <v>137.76000000000022</v>
       </c>
-      <c r="K11">
+      <c r="M11">
         <v>3013.09</v>
       </c>
-      <c r="M11" s="5" t="s">
+      <c r="O11" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="N11" s="18">
+      <c r="P11" s="18">
         <f>C20</f>
         <v>1898.28</v>
       </c>
-      <c r="O11" s="19">
-        <f t="shared" si="0"/>
+      <c r="Q11" s="19">
+        <f t="shared" si="5"/>
         <v>1.9116695245166675</v>
       </c>
-      <c r="P11" s="18">
-        <f>D20</f>
+      <c r="R11" s="18">
+        <f>F20</f>
         <v>1940.76</v>
       </c>
-      <c r="Q11" s="19">
-        <f>P11/$P$12*100</f>
+      <c r="S11" s="19">
+        <f t="shared" si="1"/>
         <v>1.884173740554181</v>
       </c>
-      <c r="R11" s="21">
-        <f>Q11-O11</f>
+      <c r="T11" s="21">
+        <f t="shared" si="2"/>
         <v>-2.7495783962486531E-2</v>
       </c>
-      <c r="S11" s="5">
-        <f>K20</f>
+      <c r="U11" s="5">
+        <f>M20</f>
         <v>1940.76</v>
       </c>
-      <c r="T11" s="22">
-        <f t="shared" si="1"/>
+      <c r="V11" s="22">
+        <f t="shared" si="6"/>
         <v>1.8836101382397239</v>
       </c>
-      <c r="U11" s="20">
-        <f>T11-O11</f>
+      <c r="W11" s="20">
+        <f t="shared" si="3"/>
         <v>-2.8059386276943599E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
         <v>44</v>
       </c>
@@ -1520,42 +1605,49 @@
       <c r="C12" s="1">
         <v>2564.64</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="1">
+        <v>9</v>
+      </c>
+      <c r="E12" s="35">
+        <f t="shared" si="4"/>
+        <v>284.95999999999998</v>
+      </c>
+      <c r="F12">
         <v>2394.27</v>
       </c>
-      <c r="E12">
-        <f>D12-C12</f>
+      <c r="G12">
+        <f t="shared" si="0"/>
         <v>-170.36999999999989</v>
       </c>
-      <c r="K12">
+      <c r="M12">
         <v>2394.27</v>
       </c>
-      <c r="N12">
-        <f>SUM(N2:N11)</f>
+      <c r="P12">
+        <f>SUM(P2:P11)</f>
         <v>99299.589999999982</v>
       </c>
-      <c r="O12">
-        <f t="shared" ref="O12:Q12" si="2">SUM(O2:O11)</f>
+      <c r="Q12">
+        <f t="shared" ref="Q12:S12" si="7">SUM(Q2:Q11)</f>
         <v>100.00000000000001</v>
       </c>
-      <c r="P12">
-        <f t="shared" si="2"/>
+      <c r="R12">
+        <f t="shared" si="7"/>
         <v>103003.23999999998</v>
       </c>
-      <c r="Q12">
-        <f t="shared" si="2"/>
+      <c r="S12">
+        <f t="shared" si="7"/>
         <v>100.00000000000004</v>
       </c>
-      <c r="S12">
-        <f>SUM(S2:S11)</f>
+      <c r="U12">
+        <f>SUM(U2:U11)</f>
         <v>103034.05999999998</v>
       </c>
-      <c r="T12">
-        <f t="shared" ref="T12" si="3">SUM(T2:T11)</f>
+      <c r="V12">
+        <f t="shared" ref="V12" si="8">SUM(V2:V11)</f>
         <v>100.00000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
         <v>44</v>
       </c>
@@ -1565,18 +1657,25 @@
       <c r="C13" s="1">
         <v>2501.8000000000002</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="1">
+        <v>7</v>
+      </c>
+      <c r="E13" s="35">
+        <f t="shared" si="4"/>
+        <v>357.40000000000003</v>
+      </c>
+      <c r="F13">
         <v>2656.08</v>
       </c>
-      <c r="E13">
-        <f>D13-C13</f>
+      <c r="G13">
+        <f t="shared" si="0"/>
         <v>154.27999999999975</v>
       </c>
-      <c r="K13">
+      <c r="M13">
         <v>2656.08</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A14" s="8" t="s">
         <v>51</v>
       </c>
@@ -1586,24 +1685,31 @@
       <c r="C14" s="1">
         <v>2289.52</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="1">
+        <v>2</v>
+      </c>
+      <c r="E14" s="35">
+        <f t="shared" si="4"/>
+        <v>1144.76</v>
+      </c>
+      <c r="F14">
         <v>2034.06</v>
       </c>
-      <c r="E14">
-        <f>D14-C14</f>
+      <c r="G14">
+        <f t="shared" si="0"/>
         <v>-255.46000000000004</v>
       </c>
-      <c r="K14">
+      <c r="M14">
         <v>2034.06</v>
       </c>
-      <c r="M14" s="23" t="s">
+      <c r="O14" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="N14" t="s">
+      <c r="P14" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A15" s="6" t="s">
         <v>45</v>
       </c>
@@ -1613,24 +1719,31 @@
       <c r="C15" s="1">
         <v>2221.1</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="1">
+        <v>5</v>
+      </c>
+      <c r="E15" s="35">
+        <f t="shared" si="4"/>
+        <v>444.21999999999997</v>
+      </c>
+      <c r="F15">
         <v>2391.15</v>
       </c>
-      <c r="E15">
-        <f>D15-C15</f>
+      <c r="G15">
+        <f t="shared" si="0"/>
         <v>170.05000000000018</v>
       </c>
-      <c r="K15">
+      <c r="M15">
         <v>2391.15</v>
       </c>
-      <c r="M15" s="27" t="s">
+      <c r="O15" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="N15" t="s">
+      <c r="P15" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A16" s="8" t="s">
         <v>51</v>
       </c>
@@ -1640,18 +1753,25 @@
       <c r="C16" s="1">
         <v>2531.3200000000002</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="1">
+        <v>4</v>
+      </c>
+      <c r="E16" s="35">
+        <f t="shared" si="4"/>
+        <v>632.83000000000004</v>
+      </c>
+      <c r="F16">
         <v>2570.04</v>
       </c>
-      <c r="E16">
-        <f>D16-C16</f>
+      <c r="G16">
+        <f t="shared" si="0"/>
         <v>38.7199999999998</v>
       </c>
-      <c r="K16">
+      <c r="M16">
         <v>2570.04</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="8" t="s">
         <v>51</v>
       </c>
@@ -1661,18 +1781,25 @@
       <c r="C17" s="1">
         <v>1956.72</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="1">
+        <v>8</v>
+      </c>
+      <c r="E17" s="35">
+        <f t="shared" si="4"/>
+        <v>244.59</v>
+      </c>
+      <c r="F17">
         <v>2091.04</v>
       </c>
-      <c r="E17">
-        <f>D17-C17</f>
+      <c r="G17">
+        <f t="shared" si="0"/>
         <v>134.31999999999994</v>
       </c>
-      <c r="K17">
+      <c r="M17">
         <v>2091.04</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="11" t="s">
         <v>52</v>
       </c>
@@ -1682,18 +1809,25 @@
       <c r="C18" s="1">
         <v>1904.95</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="1">
+        <v>5</v>
+      </c>
+      <c r="E18" s="35">
+        <f t="shared" si="4"/>
+        <v>380.99</v>
+      </c>
+      <c r="F18">
         <v>1955.3</v>
       </c>
-      <c r="E18">
-        <f>D18-C18</f>
+      <c r="G18">
+        <f t="shared" si="0"/>
         <v>50.349999999999909</v>
       </c>
-      <c r="K18">
+      <c r="M18">
         <v>1955.3</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="12" t="s">
         <v>48</v>
       </c>
@@ -1703,18 +1837,25 @@
       <c r="C19" s="1">
         <v>1918.79</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="1">
+        <v>17</v>
+      </c>
+      <c r="E19" s="35">
+        <f t="shared" si="4"/>
+        <v>112.87</v>
+      </c>
+      <c r="F19">
         <v>2011.78</v>
       </c>
-      <c r="E19">
-        <f>D19-C19</f>
+      <c r="G19">
+        <f t="shared" si="0"/>
         <v>92.990000000000009</v>
       </c>
-      <c r="K19">
+      <c r="M19">
         <v>2011.78</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" s="14" t="s">
         <v>53</v>
       </c>
@@ -1724,18 +1865,25 @@
       <c r="C20" s="1">
         <v>1898.28</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="1">
+        <v>36</v>
+      </c>
+      <c r="E20" s="35">
+        <f t="shared" si="4"/>
+        <v>52.73</v>
+      </c>
+      <c r="F20">
         <v>1940.76</v>
       </c>
-      <c r="E20">
-        <f>D20-C20</f>
+      <c r="G20">
+        <f t="shared" si="0"/>
         <v>42.480000000000018</v>
       </c>
-      <c r="K20">
+      <c r="M20">
         <v>1940.76</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" s="11" t="s">
         <v>52</v>
       </c>
@@ -1745,18 +1893,25 @@
       <c r="C21" s="1">
         <v>1906.8</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="1">
+        <v>12</v>
+      </c>
+      <c r="E21" s="35">
+        <f t="shared" si="4"/>
+        <v>158.9</v>
+      </c>
+      <c r="F21">
         <v>1917.84</v>
       </c>
-      <c r="E21">
-        <f>D21-C21</f>
+      <c r="G21">
+        <f t="shared" si="0"/>
         <v>11.039999999999964</v>
       </c>
-      <c r="K21">
+      <c r="M21">
         <v>1917.84</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" s="13" t="s">
         <v>47</v>
       </c>
@@ -1766,18 +1921,25 @@
       <c r="C22" s="1">
         <v>1837.36</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="1">
+        <v>7</v>
+      </c>
+      <c r="E22" s="35">
+        <f t="shared" si="4"/>
+        <v>262.47999999999996</v>
+      </c>
+      <c r="F22">
         <v>1907.99</v>
       </c>
-      <c r="E22">
-        <f>D22-C22</f>
+      <c r="G22">
+        <f t="shared" si="0"/>
         <v>70.630000000000109</v>
       </c>
-      <c r="K22">
+      <c r="M22">
         <v>1907.99</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" s="9" t="s">
         <v>50</v>
       </c>
@@ -1787,18 +1949,25 @@
       <c r="C23" s="1">
         <v>1805.48</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="1">
+        <v>21</v>
+      </c>
+      <c r="E23" s="35">
+        <f t="shared" si="4"/>
+        <v>85.975238095238097</v>
+      </c>
+      <c r="F23">
         <v>1890.84</v>
       </c>
-      <c r="E23">
-        <f>D23-C23</f>
+      <c r="G23">
+        <f t="shared" si="0"/>
         <v>85.3599999999999</v>
       </c>
-      <c r="K23">
+      <c r="M23">
         <v>1890.84</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" s="11" t="s">
         <v>52</v>
       </c>
@@ -1808,18 +1977,25 @@
       <c r="C24" s="1">
         <v>1735.8</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="1">
+        <v>33</v>
+      </c>
+      <c r="E24" s="35">
+        <f t="shared" si="4"/>
+        <v>52.6</v>
+      </c>
+      <c r="F24">
         <v>1794.87</v>
       </c>
-      <c r="E24">
-        <f>D24-C24</f>
+      <c r="G24">
+        <f t="shared" si="0"/>
         <v>59.069999999999936</v>
       </c>
-      <c r="K24">
+      <c r="M24">
         <v>1794.87</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" s="15" t="s">
         <v>49</v>
       </c>
@@ -1829,18 +2005,25 @@
       <c r="C25" s="1">
         <v>2849.04</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="1">
+        <v>1</v>
+      </c>
+      <c r="E25" s="35">
+        <f t="shared" si="4"/>
+        <v>2849.04</v>
+      </c>
+      <c r="F25">
         <v>2973.5</v>
       </c>
-      <c r="E25">
-        <f>D25-C25</f>
+      <c r="G25">
+        <f t="shared" si="0"/>
         <v>124.46000000000004</v>
       </c>
-      <c r="K25">
+      <c r="M25">
         <v>2973.5</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" s="7" t="s">
         <v>44</v>
       </c>
@@ -1850,18 +2033,25 @@
       <c r="C26" s="1">
         <v>1633.8</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="1">
+        <v>5</v>
+      </c>
+      <c r="E26" s="35">
+        <f t="shared" si="4"/>
+        <v>326.76</v>
+      </c>
+      <c r="F26">
         <v>1509.9</v>
       </c>
-      <c r="E26">
-        <f>D26-C26</f>
+      <c r="G26">
+        <f t="shared" si="0"/>
         <v>-123.89999999999986</v>
       </c>
-      <c r="K26">
+      <c r="M26">
         <v>1509.9</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" s="11" t="s">
         <v>52</v>
       </c>
@@ -1871,18 +2061,25 @@
       <c r="C27" s="1">
         <v>1433.4</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="1">
+        <v>30</v>
+      </c>
+      <c r="E27" s="35">
+        <f t="shared" si="4"/>
+        <v>47.78</v>
+      </c>
+      <c r="F27">
         <v>1506</v>
       </c>
-      <c r="E27">
-        <f>D27-C27</f>
+      <c r="G27">
+        <f t="shared" si="0"/>
         <v>72.599999999999909</v>
       </c>
-      <c r="K27">
+      <c r="M27">
         <v>1506</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" s="12" t="s">
         <v>48</v>
       </c>
@@ -1892,18 +2089,25 @@
       <c r="C28" s="1">
         <v>1316.48</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="1">
+        <v>22</v>
+      </c>
+      <c r="E28" s="35">
+        <f t="shared" si="4"/>
+        <v>59.84</v>
+      </c>
+      <c r="F28">
         <v>1385.56</v>
       </c>
-      <c r="E28">
-        <f>D28-C28</f>
+      <c r="G28">
+        <f t="shared" si="0"/>
         <v>69.079999999999927</v>
       </c>
-      <c r="K28">
+      <c r="M28">
         <v>1385.56</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" s="7" t="s">
         <v>44</v>
       </c>
@@ -1913,18 +2117,25 @@
       <c r="C29" s="1">
         <v>1339.7</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="1">
+        <v>2</v>
+      </c>
+      <c r="E29" s="35">
+        <f t="shared" si="4"/>
+        <v>669.85</v>
+      </c>
+      <c r="F29">
         <v>1308.9000000000001</v>
       </c>
-      <c r="E29">
-        <f>D29-C29</f>
+      <c r="G29">
+        <f t="shared" si="0"/>
         <v>-30.799999999999955</v>
       </c>
-      <c r="K29">
+      <c r="M29">
         <v>1308.9000000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" s="11" t="s">
         <v>52</v>
       </c>
@@ -1934,18 +2145,25 @@
       <c r="C30" s="1">
         <v>1218.4000000000001</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="1">
+        <v>8</v>
+      </c>
+      <c r="E30" s="35">
+        <f t="shared" si="4"/>
+        <v>152.30000000000001</v>
+      </c>
+      <c r="F30">
         <v>1336.24</v>
       </c>
-      <c r="E30">
-        <f>D30-C30</f>
+      <c r="G30">
+        <f t="shared" si="0"/>
         <v>117.83999999999992</v>
       </c>
-      <c r="K30">
+      <c r="M30">
         <v>1336.24</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" s="7" t="s">
         <v>44</v>
       </c>
@@ -1955,18 +2173,25 @@
       <c r="C31" s="1">
         <v>1206.48</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="1">
+        <v>22</v>
+      </c>
+      <c r="E31" s="35">
+        <f t="shared" si="4"/>
+        <v>54.84</v>
+      </c>
+      <c r="F31">
         <v>1303.5</v>
       </c>
-      <c r="E31">
-        <f>D31-C31</f>
+      <c r="G31">
+        <f t="shared" si="0"/>
         <v>97.019999999999982</v>
       </c>
-      <c r="K31">
+      <c r="M31">
         <v>1303.5</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" s="11" t="s">
         <v>52</v>
       </c>
@@ -1976,18 +2201,25 @@
       <c r="C32" s="1">
         <v>904.61</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="1">
+        <v>1</v>
+      </c>
+      <c r="E32" s="35">
+        <f t="shared" si="4"/>
+        <v>904.61</v>
+      </c>
+      <c r="F32">
         <v>925.13</v>
       </c>
-      <c r="E32">
-        <f>D32-C32</f>
+      <c r="G32">
+        <f t="shared" si="0"/>
         <v>20.519999999999982</v>
       </c>
-      <c r="K32">
+      <c r="M32">
         <v>925.13</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33" s="11" t="s">
         <v>52</v>
       </c>
@@ -1997,18 +2229,25 @@
       <c r="C33" s="1">
         <v>878.24</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="1">
+        <v>16</v>
+      </c>
+      <c r="E33" s="35">
+        <f t="shared" si="4"/>
+        <v>54.89</v>
+      </c>
+      <c r="F33">
         <v>907.68</v>
       </c>
-      <c r="E33">
-        <f>D33-C33</f>
+      <c r="G33">
+        <f t="shared" si="0"/>
         <v>29.439999999999941</v>
       </c>
-      <c r="K33">
+      <c r="M33">
         <v>907.68</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34" s="11" t="s">
         <v>52</v>
       </c>
@@ -2018,18 +2257,25 @@
       <c r="C34" s="1">
         <v>889.4</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="1">
+        <v>20</v>
+      </c>
+      <c r="E34" s="35">
+        <f t="shared" si="4"/>
+        <v>44.47</v>
+      </c>
+      <c r="F34">
         <v>890.4</v>
       </c>
-      <c r="E34">
-        <f>D34-C34</f>
+      <c r="G34">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K34">
+      <c r="M34">
         <v>890.4</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35" s="10" t="s">
         <v>46</v>
       </c>
@@ -2039,18 +2285,25 @@
       <c r="C35" s="1">
         <v>878.4</v>
       </c>
-      <c r="D35">
+      <c r="D35" s="1">
+        <v>10</v>
+      </c>
+      <c r="E35" s="35">
+        <f t="shared" si="4"/>
+        <v>87.84</v>
+      </c>
+      <c r="F35">
         <v>925.9</v>
       </c>
-      <c r="E35">
-        <f>D35-C35</f>
+      <c r="G35">
+        <f t="shared" si="0"/>
         <v>47.5</v>
       </c>
-      <c r="K35">
+      <c r="M35">
         <v>925.9</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A36" s="11" t="s">
         <v>52</v>
       </c>
@@ -2060,18 +2313,25 @@
       <c r="C36" s="1">
         <v>830.1</v>
       </c>
-      <c r="D36">
+      <c r="D36" s="1">
+        <v>15</v>
+      </c>
+      <c r="E36" s="35">
+        <f t="shared" si="4"/>
+        <v>55.34</v>
+      </c>
+      <c r="F36">
         <v>866.55</v>
       </c>
-      <c r="E36">
-        <f>D36-C36</f>
+      <c r="G36">
+        <f t="shared" si="0"/>
         <v>36.449999999999932</v>
       </c>
-      <c r="K36">
+      <c r="M36">
         <v>866.55</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A37" s="11" t="s">
         <v>52</v>
       </c>
@@ -2081,18 +2341,25 @@
       <c r="C37" s="1">
         <v>842.58</v>
       </c>
-      <c r="D37">
+      <c r="D37" s="1">
+        <v>6</v>
+      </c>
+      <c r="E37" s="35">
+        <f t="shared" si="4"/>
+        <v>140.43</v>
+      </c>
+      <c r="F37">
         <v>902.46</v>
       </c>
-      <c r="E37">
-        <f>D37-C37</f>
+      <c r="G37">
+        <f t="shared" si="0"/>
         <v>59.879999999999995</v>
       </c>
-      <c r="K37">
+      <c r="M37">
         <v>902.46</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A38" s="8" t="s">
         <v>51</v>
       </c>
@@ -2102,18 +2369,25 @@
       <c r="C38" s="1">
         <v>734.61</v>
       </c>
-      <c r="D38">
+      <c r="D38" s="1">
+        <v>3</v>
+      </c>
+      <c r="E38" s="35">
+        <f t="shared" si="4"/>
+        <v>244.87</v>
+      </c>
+      <c r="F38">
         <v>794.91</v>
       </c>
-      <c r="E38">
-        <f>D38-C38</f>
+      <c r="G38">
+        <f t="shared" si="0"/>
         <v>60.299999999999955</v>
       </c>
-      <c r="K38">
+      <c r="M38">
         <v>794.91</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A39" s="11" t="s">
         <v>52</v>
       </c>
@@ -2123,18 +2397,25 @@
       <c r="C39" s="1">
         <v>586.6</v>
       </c>
-      <c r="D39">
+      <c r="D39" s="1">
+        <v>10</v>
+      </c>
+      <c r="E39" s="35">
+        <f t="shared" si="4"/>
+        <v>58.660000000000004</v>
+      </c>
+      <c r="F39">
         <v>606.29999999999995</v>
       </c>
-      <c r="E39">
-        <f>D39-C39</f>
+      <c r="G39">
+        <f t="shared" si="0"/>
         <v>19.699999999999932</v>
       </c>
-      <c r="K39">
+      <c r="M39">
         <v>606.29999999999995</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A40" s="10" t="s">
         <v>46</v>
       </c>
@@ -2144,18 +2425,25 @@
       <c r="C40" s="1">
         <v>595.11</v>
       </c>
-      <c r="D40">
+      <c r="D40" s="1">
+        <v>3</v>
+      </c>
+      <c r="E40" s="35">
+        <f t="shared" si="4"/>
+        <v>198.37</v>
+      </c>
+      <c r="F40">
         <v>627.33000000000004</v>
       </c>
-      <c r="E40">
-        <f>D40-C40</f>
+      <c r="G40">
+        <f t="shared" si="0"/>
         <v>32.220000000000027</v>
       </c>
-      <c r="K40">
+      <c r="M40">
         <v>627.33000000000004</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A41" s="11" t="s">
         <v>52</v>
       </c>
@@ -2165,18 +2453,25 @@
       <c r="C41" s="1">
         <v>190.05</v>
       </c>
-      <c r="D41">
+      <c r="D41" s="1">
+        <v>2</v>
+      </c>
+      <c r="E41" s="35">
+        <f t="shared" si="4"/>
+        <v>95.025000000000006</v>
+      </c>
+      <c r="F41">
         <v>196.76</v>
       </c>
-      <c r="E41">
-        <f>D41-C41</f>
+      <c r="G41">
+        <f t="shared" si="0"/>
         <v>6.7099999999999795</v>
       </c>
-      <c r="K41">
+      <c r="M41">
         <v>196.76</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A42" s="9" t="s">
         <v>50</v>
       </c>
@@ -2186,18 +2481,25 @@
       <c r="C42" s="1">
         <v>243.84</v>
       </c>
-      <c r="D42">
+      <c r="D42" s="1">
+        <v>1</v>
+      </c>
+      <c r="E42" s="35">
+        <f t="shared" si="4"/>
+        <v>243.84</v>
+      </c>
+      <c r="F42">
         <v>238.18</v>
       </c>
-      <c r="E42">
-        <f>D42-C42</f>
+      <c r="G42">
+        <f t="shared" si="0"/>
         <v>-5.6599999999999966</v>
       </c>
-      <c r="K42">
+      <c r="M42">
         <v>238.18</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A43" s="6" t="s">
         <v>45</v>
       </c>
@@ -2207,34 +2509,41 @@
       <c r="C43" s="1">
         <v>178.12</v>
       </c>
-      <c r="D43">
+      <c r="D43" s="1">
+        <v>2</v>
+      </c>
+      <c r="E43" s="35">
+        <f t="shared" si="4"/>
+        <v>89.06</v>
+      </c>
+      <c r="F43">
         <v>197.74</v>
       </c>
-      <c r="E43">
-        <f>D43-C43</f>
+      <c r="G43">
+        <f t="shared" si="0"/>
         <v>19.620000000000005</v>
       </c>
-      <c r="K43">
+      <c r="M43">
         <v>197.74</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C44" s="1">
         <f>SUM(C2:C43)</f>
         <v>99299.589999999967</v>
       </c>
-      <c r="D44" s="1">
-        <f>SUM(D2:D43)</f>
+      <c r="F44" s="1">
+        <f>SUM(F2:F43)</f>
         <v>103003.23999999996</v>
       </c>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
-      <c r="K44" s="1">
-        <f>SUM(K2:K43)</f>
+      <c r="K44" s="1"/>
+      <c r="L44" s="1"/>
+      <c r="M44" s="1">
+        <f>SUM(M2:M43)</f>
         <v>103034.05999999995</v>
       </c>
     </row>

</xml_diff>